<commit_message>
Units in Excel Workbook adapted + errors fixed.
</commit_message>
<xml_diff>
--- a/ZoKBenchWorkbook.xlsx
+++ b/ZoKBenchWorkbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobeberhardt/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobeberhardt/Desktop/ZoKratesBenchmarks/exports/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EF8204-E405-C544-A36A-4AD99311D8BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41469C99-40B2-484A-98B3-13FC771379D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="49060" windowHeight="24280" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,52 +134,55 @@
     <t>File (lookup key)</t>
   </si>
   <si>
-    <t>time compilation optimized [µs]</t>
-  </si>
-  <si>
-    <t>time setup optimized [µs]</t>
-  </si>
-  <si>
-    <t>memory compilation optimized  [KiB]</t>
-  </si>
-  <si>
-    <t>memory setup optimized [KiB]</t>
-  </si>
-  <si>
-    <t>time witness-gen optimized [µs]</t>
-  </si>
-  <si>
-    <t>time proof-gen optimized [µs]</t>
-  </si>
-  <si>
-    <t>memory proof-gen  optimized [KiB]</t>
-  </si>
-  <si>
-    <t>memory  witness-gen optimized  [KiB]</t>
-  </si>
-  <si>
     <t># constraints optimized</t>
   </si>
   <si>
     <t># constraint unoptimized</t>
   </si>
   <si>
-    <t>time compilation unoptimized [µs]</t>
-  </si>
-  <si>
-    <t>time setup unoptimized [µs]</t>
-  </si>
-  <si>
-    <t>time witness-gen unoptimized [µs]</t>
-  </si>
-  <si>
-    <t>time proof-gen unoptimized [µs]</t>
+    <t>time compilation optimized [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memory compilation optimized  [MiB] </t>
+  </si>
+  <si>
+    <t>time setup optimized [s]</t>
+  </si>
+  <si>
+    <t>memory setup optimized [MiB]</t>
+  </si>
+  <si>
+    <t>time witness-gen optimized [s]</t>
+  </si>
+  <si>
+    <t>memory  witness-gen optimized  [MiB]</t>
+  </si>
+  <si>
+    <t>time proof-gen optimized [s]</t>
+  </si>
+  <si>
+    <t>memory proof-gen  optimized [MiB]</t>
+  </si>
+  <si>
+    <t>time compilation unoptimized [s]</t>
+  </si>
+  <si>
+    <t>time setup unoptimized [s]</t>
+  </si>
+  <si>
+    <t>time witness-gen unoptimized [s]</t>
+  </si>
+  <si>
+    <t>time proof-gen unoptimized [s]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -684,13 +687,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1795,10 +1799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90ECF5BE-0EC9-8846-B3D2-CDC215E09220}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1819,16 +1823,16 @@
         <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1838,21 +1842,21 @@
       <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2">
-        <f>VLOOKUP($A2,raw!$A:$S,2,FALSE)</f>
-        <v>1062259</v>
-      </c>
-      <c r="D2">
-        <f>VLOOKUP($A2,raw!$A:$S,3,FALSE)</f>
-        <v>14920</v>
-      </c>
-      <c r="E2">
-        <f>VLOOKUP($A2,raw!$A:$S,4,FALSE)</f>
-        <v>31274568</v>
-      </c>
-      <c r="F2">
-        <f>VLOOKUP($A2,raw!$A:$S,5,FALSE)</f>
-        <v>126468</v>
+      <c r="C2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>1.0622590000000001</v>
+      </c>
+      <c r="D2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>14.5703125</v>
+      </c>
+      <c r="E2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>31.274567999999999</v>
+      </c>
+      <c r="F2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>123.50390625</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1862,21 +1866,21 @@
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3">
-        <f>VLOOKUP($A3,raw!$A:$S,2,FALSE)</f>
-        <v>23112211</v>
-      </c>
-      <c r="D3">
-        <f>VLOOKUP($A3,raw!$A:$S,3,FALSE)</f>
-        <v>51076</v>
-      </c>
-      <c r="E3">
-        <f>VLOOKUP($A3,raw!$A:$S,4,FALSE)</f>
-        <v>911445394</v>
-      </c>
-      <c r="F3">
-        <f>VLOOKUP($A3,raw!$A:$S,5,FALSE)</f>
-        <v>3130440</v>
+      <c r="C3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>23.112210999999999</v>
+      </c>
+      <c r="D3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>49.87890625</v>
+      </c>
+      <c r="E3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>911.44539399999996</v>
+      </c>
+      <c r="F3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>3057.0703125</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1886,21 +1890,21 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
-        <f>VLOOKUP($A4,raw!$A:$S,2,FALSE)</f>
-        <v>26026357</v>
-      </c>
-      <c r="D4">
-        <f>VLOOKUP($A4,raw!$A:$S,3,FALSE)</f>
-        <v>12240</v>
-      </c>
-      <c r="E4">
-        <f>VLOOKUP($A4,raw!$A:$S,4,FALSE)</f>
-        <v>961483761</v>
-      </c>
-      <c r="F4">
-        <f>VLOOKUP($A4,raw!$A:$S,5,FALSE)</f>
-        <v>3385884</v>
+      <c r="C4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>26.026357000000001</v>
+      </c>
+      <c r="D4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>11.953125</v>
+      </c>
+      <c r="E4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>961.48376099999996</v>
+      </c>
+      <c r="F4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>3306.52734375</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1910,21 +1914,21 @@
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
-        <f>VLOOKUP($A5,raw!$A:$S,2,FALSE)</f>
-        <v>11202946</v>
-      </c>
-      <c r="D5">
-        <f>VLOOKUP($A5,raw!$A:$S,3,FALSE)</f>
-        <v>4124</v>
-      </c>
-      <c r="E5">
-        <f>VLOOKUP($A5,raw!$A:$S,4,FALSE)</f>
-        <v>445769364</v>
-      </c>
-      <c r="F5">
-        <f>VLOOKUP($A5,raw!$A:$S,5,FALSE)</f>
-        <v>1565036</v>
+      <c r="C5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>11.202946000000001</v>
+      </c>
+      <c r="D5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>4.02734375</v>
+      </c>
+      <c r="E5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>445.769364</v>
+      </c>
+      <c r="F5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>1528.35546875</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1934,21 +1938,21 @@
       <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C6">
-        <f>VLOOKUP($A6,raw!$A:$S,2,FALSE)</f>
-        <v>1365747</v>
-      </c>
-      <c r="D6">
-        <f>VLOOKUP($A6,raw!$A:$S,3,FALSE)</f>
-        <v>45612</v>
-      </c>
-      <c r="E6">
-        <f>VLOOKUP($A6,raw!$A:$S,4,FALSE)</f>
-        <v>38194351</v>
-      </c>
-      <c r="F6">
-        <f>VLOOKUP($A6,raw!$A:$S,5,FALSE)</f>
-        <v>148304</v>
+      <c r="C6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>1.365747</v>
+      </c>
+      <c r="D6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>44.54296875</v>
+      </c>
+      <c r="E6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>38.194350999999997</v>
+      </c>
+      <c r="F6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>144.828125</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1958,21 +1962,21 @@
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7">
-        <f>VLOOKUP($A7,raw!$A:$S,2,FALSE)</f>
-        <v>11696284</v>
-      </c>
-      <c r="D7">
-        <f>VLOOKUP($A7,raw!$A:$S,3,FALSE)</f>
-        <v>3932432</v>
-      </c>
-      <c r="E7">
-        <f>VLOOKUP($A7,raw!$A:$S,4,FALSE)</f>
-        <v>459151206</v>
-      </c>
-      <c r="F7">
-        <f>VLOOKUP($A7,raw!$A:$S,5,FALSE)</f>
-        <v>1576996</v>
+      <c r="C7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>11.696284</v>
+      </c>
+      <c r="D7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>3840.265625</v>
+      </c>
+      <c r="E7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>459.151206</v>
+      </c>
+      <c r="F7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>1540.03515625</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1982,127 +1986,124 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8">
-        <f>VLOOKUP($A8,raw!$A:$S,2,FALSE)</f>
-        <v>11452208</v>
-      </c>
-      <c r="D8">
-        <f>VLOOKUP($A8,raw!$A:$S,3,FALSE)</f>
-        <v>13580</v>
-      </c>
-      <c r="E8">
-        <f>VLOOKUP($A8,raw!$A:$S,4,FALSE)</f>
-        <v>451959024</v>
-      </c>
-      <c r="F8">
-        <f>VLOOKUP($A8,raw!$A:$S,5,FALSE)</f>
-        <v>1583856</v>
+      <c r="C8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>11.452208000000001</v>
+      </c>
+      <c r="D8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>13.26171875</v>
+      </c>
+      <c r="E8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>451.959024</v>
+      </c>
+      <c r="F8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>1546.734375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>2.474818</v>
+      </c>
+      <c r="D9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>3306.52734375</v>
+      </c>
+      <c r="E9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>79.102241000000006</v>
+      </c>
+      <c r="F9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>308.07421875</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10">
-        <f>VLOOKUP($A10,raw!$A:$S,2,FALSE)</f>
-        <v>2474818</v>
-      </c>
-      <c r="D10">
-        <f>VLOOKUP($A10,raw!$A:$S,3,FALSE)</f>
-        <v>3385884</v>
-      </c>
-      <c r="E10">
-        <f>VLOOKUP($A10,raw!$A:$S,4,FALSE)</f>
-        <v>79102241</v>
-      </c>
-      <c r="F10">
-        <f>VLOOKUP($A10,raw!$A:$S,5,FALSE)</f>
-        <v>315468</v>
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>0.76018399999999997</v>
+      </c>
+      <c r="D10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>1686.2265625</v>
+      </c>
+      <c r="E10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>19.229776999999999</v>
+      </c>
+      <c r="F10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>76.76953125</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>1.811952</v>
+      </c>
+      <c r="D11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>32.5234375</v>
+      </c>
+      <c r="E11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>2.0795149999999998</v>
+      </c>
+      <c r="F11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>11.953125</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <f>VLOOKUP($A12,raw!$A:$S,2,FALSE)</f>
-        <v>760184</v>
-      </c>
-      <c r="D12">
-        <f>VLOOKUP($A12,raw!$A:$S,3,FALSE)</f>
-        <v>1726696</v>
-      </c>
-      <c r="E12">
-        <f>VLOOKUP($A12,raw!$A:$S,4,FALSE)</f>
-        <v>19229777</v>
-      </c>
-      <c r="F12">
-        <f>VLOOKUP($A12,raw!$A:$S,5,FALSE)</f>
-        <v>78612</v>
+        <v>30</v>
+      </c>
+      <c r="C12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>7.8250539999999997</v>
+      </c>
+      <c r="D12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,3,FALSE) / (1024)</f>
+        <v>29.7578125</v>
+      </c>
+      <c r="E12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>0.98872099999999996</v>
+      </c>
+      <c r="F12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,5,FALSE)/(1024)</f>
+        <v>21.95703125</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13">
-        <f>VLOOKUP($A13,raw!$A:$S,2,FALSE)</f>
-        <v>1811952</v>
-      </c>
-      <c r="D13">
-        <f>VLOOKUP($A13,raw!$A:$S,3,FALSE)</f>
-        <v>33304</v>
-      </c>
-      <c r="E13">
-        <f>VLOOKUP($A13,raw!$A:$S,4,FALSE)</f>
-        <v>2079515</v>
-      </c>
-      <c r="F13">
-        <f>VLOOKUP($A13,raw!$A:$S,5,FALSE)</f>
-        <v>12240</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14">
-        <f>VLOOKUP($A14,raw!$A:$S,2,FALSE)</f>
-        <v>7825054</v>
-      </c>
-      <c r="D14">
-        <f>VLOOKUP($A14,raw!$A:$S,3,FALSE)</f>
-        <v>30472</v>
-      </c>
-      <c r="E14">
-        <f>VLOOKUP($A14,raw!$A:$S,4,FALSE)</f>
-        <v>988721</v>
-      </c>
-      <c r="F14">
-        <f>VLOOKUP($A14,raw!$A:$S,5,FALSE)</f>
-        <v>22484</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C30" s="4"/>
+      <c r="A13" s="3"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2111,10 +2112,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66151232-E4E7-5748-9B3D-48CAC8B6C313}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2123,8 +2124,8 @@
     <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2135,16 +2136,16 @@
         <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2154,21 +2155,21 @@
       <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2">
-        <f>VLOOKUP($A2,raw!$A:$S,6,FALSE)</f>
-        <v>558919</v>
-      </c>
-      <c r="D2">
-        <f>VLOOKUP($A2,raw!$A:$S,7,FALSE)</f>
-        <v>64324</v>
-      </c>
-      <c r="E2">
-        <f>VLOOKUP($A2,raw!$A:$S,8,FALSE)</f>
-        <v>3585537</v>
-      </c>
-      <c r="F2">
-        <f>VLOOKUP($A2,raw!$A:$S,9,FALSE)</f>
-        <v>226792</v>
+      <c r="C2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>0.55891900000000005</v>
+      </c>
+      <c r="D2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>62.81640625</v>
+      </c>
+      <c r="E2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>3.585537</v>
+      </c>
+      <c r="F2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>221.4765625</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2178,21 +2179,21 @@
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3">
-        <f>VLOOKUP($A3,raw!$A:$S,6,FALSE)</f>
-        <v>9499208</v>
-      </c>
-      <c r="D3">
-        <f>VLOOKUP($A3,raw!$A:$S,7,FALSE)</f>
-        <v>1567660</v>
-      </c>
-      <c r="E3">
-        <f>VLOOKUP($A3,raw!$A:$S,8,FALSE)</f>
-        <v>99552277</v>
-      </c>
-      <c r="F3">
-        <f>VLOOKUP($A3,raw!$A:$S,9,FALSE)</f>
-        <v>6159112</v>
+      <c r="C3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>9.4992079999999994</v>
+      </c>
+      <c r="D3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>1530.91796875</v>
+      </c>
+      <c r="E3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>99.552277000000004</v>
+      </c>
+      <c r="F3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>6014.7578125</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2202,21 +2203,21 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
-        <f>VLOOKUP($A4,raw!$A:$S,6,FALSE)</f>
-        <v>11125174</v>
-      </c>
-      <c r="D4">
-        <f>VLOOKUP($A4,raw!$A:$S,7,FALSE)</f>
-        <v>1726696</v>
-      </c>
-      <c r="E4">
-        <f>VLOOKUP($A4,raw!$A:$S,8,FALSE)</f>
-        <v>103534028</v>
-      </c>
-      <c r="F4">
-        <f>VLOOKUP($A4,raw!$A:$S,9,FALSE)</f>
-        <v>6728188</v>
+      <c r="C4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>11.125173999999999</v>
+      </c>
+      <c r="D4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>1686.2265625</v>
+      </c>
+      <c r="E4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>103.53402800000001</v>
+      </c>
+      <c r="F4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>6570.49609375</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2226,21 +2227,21 @@
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
-        <f>VLOOKUP($A5,raw!$A:$S,6,FALSE)</f>
-        <v>4719280</v>
-      </c>
-      <c r="D5">
-        <f>VLOOKUP($A5,raw!$A:$S,7,FALSE)</f>
-        <v>768652</v>
-      </c>
-      <c r="E5">
-        <f>VLOOKUP($A5,raw!$A:$S,8,FALSE)</f>
-        <v>48942751</v>
-      </c>
-      <c r="F5">
-        <f>VLOOKUP($A5,raw!$A:$S,9,FALSE)</f>
-        <v>3014660</v>
+      <c r="C5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>4.7192800000000004</v>
+      </c>
+      <c r="D5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>750.63671875</v>
+      </c>
+      <c r="E5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>48.942751000000001</v>
+      </c>
+      <c r="F5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>2944.00390625</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2250,21 +2251,21 @@
       <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C6">
-        <f>VLOOKUP($A6,raw!$A:$S,6,FALSE)</f>
-        <v>659943</v>
-      </c>
-      <c r="D6">
-        <f>VLOOKUP($A6,raw!$A:$S,7,FALSE)</f>
-        <v>83020</v>
-      </c>
-      <c r="E6">
-        <f>VLOOKUP($A6,raw!$A:$S,8,FALSE)</f>
-        <v>4037975</v>
-      </c>
-      <c r="F6">
-        <f>VLOOKUP($A6,raw!$A:$S,9,FALSE)</f>
-        <v>293544</v>
+      <c r="C6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>0.65994299999999995</v>
+      </c>
+      <c r="D6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>81.07421875</v>
+      </c>
+      <c r="E6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>4.0379750000000003</v>
+      </c>
+      <c r="F6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>286.6640625</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2274,21 +2275,21 @@
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7">
-        <f>VLOOKUP($A7,raw!$A:$S,6,FALSE)</f>
-        <v>4933268</v>
-      </c>
-      <c r="D7">
-        <f>VLOOKUP($A7,raw!$A:$S,7,FALSE)</f>
-        <v>806820</v>
-      </c>
-      <c r="E7">
-        <f>VLOOKUP($A7,raw!$A:$S,8,FALSE)</f>
-        <v>49631498</v>
-      </c>
-      <c r="F7">
-        <f>VLOOKUP($A7,raw!$A:$S,9,FALSE)</f>
-        <v>3188368</v>
+      <c r="C7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>4.933268</v>
+      </c>
+      <c r="D7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>787.91015625</v>
+      </c>
+      <c r="E7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>49.631498000000001</v>
+      </c>
+      <c r="F7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>3113.640625</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2298,120 +2299,117 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8">
-        <f>VLOOKUP($A8,raw!$A:$S,6,FALSE)</f>
-        <v>4801734</v>
-      </c>
-      <c r="D8">
-        <f>VLOOKUP($A8,raw!$A:$S,7,FALSE)</f>
-        <v>787272</v>
-      </c>
-      <c r="E8">
-        <f>VLOOKUP($A8,raw!$A:$S,8,FALSE)</f>
-        <v>49143239</v>
-      </c>
-      <c r="F8">
-        <f>VLOOKUP($A8,raw!$A:$S,9,FALSE)</f>
-        <v>3081448</v>
+      <c r="C8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>4.8017339999999997</v>
+      </c>
+      <c r="D8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>768.8203125</v>
+      </c>
+      <c r="E8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>49.143239000000001</v>
+      </c>
+      <c r="F8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>3009.2265625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>1.164191</v>
+      </c>
+      <c r="D9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>158.1953125</v>
+      </c>
+      <c r="E9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>8.1751839999999998</v>
+      </c>
+      <c r="F9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>582.171875</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10">
-        <f>VLOOKUP($A10,raw!$A:$S,6,FALSE)</f>
-        <v>1164191</v>
-      </c>
-      <c r="D10">
-        <f>VLOOKUP($A10,raw!$A:$S,7,FALSE)</f>
-        <v>161992</v>
-      </c>
-      <c r="E10">
-        <f>VLOOKUP($A10,raw!$A:$S,8,FALSE)</f>
-        <v>8175184</v>
-      </c>
-      <c r="F10">
-        <f>VLOOKUP($A10,raw!$A:$S,9,FALSE)</f>
-        <v>596144</v>
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>0.41484199999999999</v>
+      </c>
+      <c r="D10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>43.8203125</v>
+      </c>
+      <c r="E10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>2.184739</v>
+      </c>
+      <c r="F10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>147.01171875</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>0.26312099999999999</v>
+      </c>
+      <c r="D11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>4.02734375</v>
+      </c>
+      <c r="E11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>0.82185900000000001</v>
+      </c>
+      <c r="F11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>14.5703125</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <f>VLOOKUP($A12,raw!$A:$S,6,FALSE)</f>
-        <v>414842</v>
-      </c>
-      <c r="D12">
-        <f>VLOOKUP($A12,raw!$A:$S,7,FALSE)</f>
-        <v>44872</v>
-      </c>
-      <c r="E12">
-        <f>VLOOKUP($A12,raw!$A:$S,8,FALSE)</f>
-        <v>2184739</v>
-      </c>
-      <c r="F12">
-        <f>VLOOKUP($A12,raw!$A:$S,9,FALSE)</f>
-        <v>150540</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13">
-        <f>VLOOKUP($A13,raw!$A:$S,6,FALSE)</f>
-        <v>263121</v>
-      </c>
-      <c r="D13">
-        <f>VLOOKUP($A13,raw!$A:$S,7,FALSE)</f>
-        <v>4124</v>
-      </c>
-      <c r="E13">
-        <f>VLOOKUP($A13,raw!$A:$S,8,FALSE)</f>
-        <v>821859</v>
-      </c>
-      <c r="F13">
-        <f>VLOOKUP($A13,raw!$A:$S,9,FALSE)</f>
-        <v>14920</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14">
-        <f>VLOOKUP($A14,raw!$A:$S,6,FALSE)</f>
-        <v>255698</v>
-      </c>
-      <c r="D14">
-        <f>VLOOKUP($A14,raw!$A:$S,7,FALSE)</f>
-        <v>4888</v>
-      </c>
-      <c r="E14">
-        <f>VLOOKUP($A14,raw!$A:$S,8,FALSE)</f>
-        <v>465568</v>
-      </c>
-      <c r="F14">
-        <f>VLOOKUP($A14,raw!$A:$S,9,FALSE)</f>
-        <v>39348</v>
+      <c r="C12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>0.25569799999999998</v>
+      </c>
+      <c r="D12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,7,FALSE)/(1024)</f>
+        <v>4.7734375</v>
+      </c>
+      <c r="E12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>0.46556799999999998</v>
+      </c>
+      <c r="F12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,9,FALSE)/(1024)</f>
+        <v>38.42578125</v>
       </c>
     </row>
   </sheetData>
@@ -2421,10 +2419,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA49891-3239-0F49-8FFF-87FC4289CF2F}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2451,31 +2449,31 @@
         <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>46</v>
@@ -2496,37 +2494,37 @@
         <f>VLOOKUP($A2,raw!$A:$S,18,FALSE)</f>
         <v>257980</v>
       </c>
-      <c r="E2">
-        <f>VLOOKUP($A2,raw!$A:$S,2,FALSE)</f>
-        <v>1062259</v>
-      </c>
-      <c r="F2">
-        <f>VLOOKUP($A2,raw!$A:$S,11,FALSE)</f>
-        <v>609323</v>
-      </c>
-      <c r="G2">
-        <f>VLOOKUP($A2,raw!$A:$S,4,FALSE)</f>
-        <v>31274568</v>
-      </c>
-      <c r="H2">
-        <f>VLOOKUP($A2,raw!$A:$S,13,FALSE)</f>
-        <v>38158295</v>
-      </c>
-      <c r="I2">
-        <f>VLOOKUP($A2,raw!$A:$S,7,FALSE)</f>
-        <v>64324</v>
-      </c>
-      <c r="J2">
-        <f>VLOOKUP($A2,raw!$A:$S,16,FALSE)</f>
-        <v>71404</v>
-      </c>
-      <c r="K2">
-        <f>VLOOKUP($A2,raw!$A:$S,8,FALSE)</f>
-        <v>3585537</v>
-      </c>
-      <c r="L2">
-        <f>VLOOKUP($A2,raw!$A:$S,17,FALSE)</f>
-        <v>3839166</v>
+      <c r="E2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>1.0622590000000001</v>
+      </c>
+      <c r="F2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>0.60932299999999995</v>
+      </c>
+      <c r="G2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>31.274567999999999</v>
+      </c>
+      <c r="H2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>38.158295000000003</v>
+      </c>
+      <c r="I2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>0.55891900000000005</v>
+      </c>
+      <c r="J2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>0.55914799999999998</v>
+      </c>
+      <c r="K2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>3.585537</v>
+      </c>
+      <c r="L2" s="6">
+        <f>VLOOKUP($A2,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>3.8391660000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2544,37 +2542,37 @@
         <f>VLOOKUP($A3,raw!$A:$S,18,FALSE)</f>
         <v>7544412</v>
       </c>
-      <c r="E3">
-        <f>VLOOKUP($A3,raw!$A:$S,2,FALSE)</f>
-        <v>23112211</v>
-      </c>
-      <c r="F3">
-        <f>VLOOKUP($A3,raw!$A:$S,11,FALSE)</f>
-        <v>9340337</v>
-      </c>
-      <c r="G3">
-        <f>VLOOKUP($A3,raw!$A:$S,4,FALSE)</f>
-        <v>911445394</v>
-      </c>
-      <c r="H3">
-        <f>VLOOKUP($A3,raw!$A:$S,13,FALSE)</f>
-        <v>1188147590</v>
-      </c>
-      <c r="I3">
-        <f>VLOOKUP($A3,raw!$A:$S,7,FALSE)</f>
-        <v>1567660</v>
-      </c>
-      <c r="J3">
-        <f>VLOOKUP($A3,raw!$A:$S,16,FALSE)</f>
-        <v>1866852</v>
-      </c>
-      <c r="K3">
-        <f>VLOOKUP($A3,raw!$A:$S,9,FALSE)</f>
-        <v>6159112</v>
-      </c>
-      <c r="L3">
-        <f>VLOOKUP($A3,raw!$A:$S,17,FALSE)</f>
-        <v>106763190</v>
+      <c r="E3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>23.112210999999999</v>
+      </c>
+      <c r="F3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>9.3403369999999999</v>
+      </c>
+      <c r="G3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>911.44539399999996</v>
+      </c>
+      <c r="H3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>1188.14759</v>
+      </c>
+      <c r="I3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>9.4992079999999994</v>
+      </c>
+      <c r="J3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>11.307957</v>
+      </c>
+      <c r="K3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>99.552277000000004</v>
+      </c>
+      <c r="L3" s="6">
+        <f>VLOOKUP($A3,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>106.76318999999999</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2592,37 +2590,37 @@
         <f>VLOOKUP($A4,raw!$A:$S,18,FALSE)</f>
         <v>8172896</v>
       </c>
-      <c r="E4">
-        <f>VLOOKUP($A4,raw!$A:$S,2,FALSE)</f>
-        <v>26026357</v>
-      </c>
-      <c r="F4">
-        <f>VLOOKUP($A4,raw!$A:$S,11,FALSE)</f>
-        <v>10392279</v>
-      </c>
-      <c r="G4">
-        <f>VLOOKUP($A4,raw!$A:$S,4,FALSE)</f>
-        <v>961483761</v>
-      </c>
-      <c r="H4">
-        <f>VLOOKUP($A4,raw!$A:$S,13,FALSE)</f>
-        <v>1230247608</v>
-      </c>
-      <c r="I4">
-        <f>VLOOKUP($A4,raw!$A:$S,7,FALSE)</f>
-        <v>1726696</v>
-      </c>
-      <c r="J4">
-        <f>VLOOKUP($A4,raw!$A:$S,16,FALSE)</f>
-        <v>2015604</v>
-      </c>
-      <c r="K4">
-        <f>VLOOKUP($A4,raw!$A:$S,9,FALSE)</f>
-        <v>6728188</v>
-      </c>
-      <c r="L4">
-        <f>VLOOKUP($A4,raw!$A:$S,17,FALSE)</f>
-        <v>110844067</v>
+      <c r="E4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>26.026357000000001</v>
+      </c>
+      <c r="F4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>10.392279</v>
+      </c>
+      <c r="G4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>961.48376099999996</v>
+      </c>
+      <c r="H4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>1230.2476079999999</v>
+      </c>
+      <c r="I4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>11.125173999999999</v>
+      </c>
+      <c r="J4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>12.896936</v>
+      </c>
+      <c r="K4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>103.53402800000001</v>
+      </c>
+      <c r="L4" s="6">
+        <f>VLOOKUP($A4,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>110.844067</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2640,37 +2638,37 @@
         <f>VLOOKUP($A5,raw!$A:$S,18,FALSE)</f>
         <v>3701396</v>
       </c>
-      <c r="E5">
-        <f>VLOOKUP($A5,raw!$A:$S,2,FALSE)</f>
-        <v>11202946</v>
-      </c>
-      <c r="F5">
-        <f>VLOOKUP($A5,raw!$A:$S,11,FALSE)</f>
-        <v>4732654</v>
-      </c>
-      <c r="G5">
-        <f>VLOOKUP($A5,raw!$A:$S,4,FALSE)</f>
-        <v>445769364</v>
-      </c>
-      <c r="H5">
-        <f>VLOOKUP($A5,raw!$A:$S,13,FALSE)</f>
-        <v>585935403</v>
-      </c>
-      <c r="I5">
-        <f>VLOOKUP($A5,raw!$A:$S,7,FALSE)</f>
-        <v>768652</v>
-      </c>
-      <c r="J5">
-        <f>VLOOKUP($A5,raw!$A:$S,16,FALSE)</f>
-        <v>917068</v>
-      </c>
-      <c r="K5">
-        <f>VLOOKUP($A5,raw!$A:$S,9,FALSE)</f>
-        <v>3014660</v>
-      </c>
-      <c r="L5">
-        <f>VLOOKUP($A5,raw!$A:$S,17,FALSE)</f>
-        <v>53393567</v>
+      <c r="E5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>11.202946000000001</v>
+      </c>
+      <c r="F5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>4.7326540000000001</v>
+      </c>
+      <c r="G5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>445.769364</v>
+      </c>
+      <c r="H5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>585.93540299999995</v>
+      </c>
+      <c r="I5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>4.7192800000000004</v>
+      </c>
+      <c r="J5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>5.6101039999999998</v>
+      </c>
+      <c r="K5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>48.942751000000001</v>
+      </c>
+      <c r="L5" s="6">
+        <f>VLOOKUP($A5,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>53.393566999999997</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -2688,37 +2686,37 @@
         <f>VLOOKUP($A6,raw!$A:$S,18,FALSE)</f>
         <v>344692</v>
       </c>
-      <c r="E6">
-        <f>VLOOKUP($A6,raw!$A:$S,2,FALSE)</f>
-        <v>1365747</v>
-      </c>
-      <c r="F6">
-        <f>VLOOKUP($A6,raw!$A:$S,11,FALSE)</f>
-        <v>709741</v>
-      </c>
-      <c r="G6">
-        <f>VLOOKUP($A6,raw!$A:$S,4,FALSE)</f>
-        <v>38194351</v>
-      </c>
-      <c r="H6">
-        <f>VLOOKUP($A6,raw!$A:$S,13,FALSE)</f>
-        <v>55245346</v>
-      </c>
-      <c r="I6">
-        <f>VLOOKUP($A6,raw!$A:$S,7,FALSE)</f>
-        <v>83020</v>
-      </c>
-      <c r="J6">
-        <f>VLOOKUP($A6,raw!$A:$S,16,FALSE)</f>
-        <v>90168</v>
-      </c>
-      <c r="K6">
-        <f>VLOOKUP($A6,raw!$A:$S,9,FALSE)</f>
-        <v>293544</v>
-      </c>
-      <c r="L6">
-        <f>VLOOKUP($A6,raw!$A:$S,17,FALSE)</f>
-        <v>6165409</v>
+      <c r="E6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>1.365747</v>
+      </c>
+      <c r="F6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>0.70974099999999996</v>
+      </c>
+      <c r="G6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>38.194350999999997</v>
+      </c>
+      <c r="H6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>55.245345999999998</v>
+      </c>
+      <c r="I6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>0.65994299999999995</v>
+      </c>
+      <c r="J6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>0.68664000000000003</v>
+      </c>
+      <c r="K6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>4.0379750000000003</v>
+      </c>
+      <c r="L6" s="6">
+        <f>VLOOKUP($A6,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>6.1654090000000004</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2736,37 +2734,37 @@
         <f>VLOOKUP($A7,raw!$A:$S,18,FALSE)</f>
         <v>3801212</v>
       </c>
-      <c r="E7">
-        <f>VLOOKUP($A7,raw!$A:$S,2,FALSE)</f>
-        <v>11696284</v>
-      </c>
-      <c r="F7">
-        <f>VLOOKUP($A7,raw!$A:$S,11,FALSE)</f>
-        <v>4929715</v>
-      </c>
-      <c r="G7">
-        <f>VLOOKUP($A7,raw!$A:$S,4,FALSE)</f>
-        <v>459151206</v>
-      </c>
-      <c r="H7">
-        <f>VLOOKUP($A7,raw!$A:$S,13,FALSE)</f>
-        <v>602441827</v>
-      </c>
-      <c r="I7">
-        <f>VLOOKUP($A7,raw!$A:$S,7,FALSE)</f>
-        <v>806820</v>
-      </c>
-      <c r="J7">
-        <f>VLOOKUP($A7,raw!$A:$S,16,FALSE)</f>
-        <v>957284</v>
-      </c>
-      <c r="K7">
-        <f>VLOOKUP($A7,raw!$A:$S,9,FALSE)</f>
-        <v>3188368</v>
-      </c>
-      <c r="L7">
-        <f>VLOOKUP($A7,raw!$A:$S,17,FALSE)</f>
-        <v>54529333</v>
+      <c r="E7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>11.696284</v>
+      </c>
+      <c r="F7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>4.9297149999999998</v>
+      </c>
+      <c r="G7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>459.151206</v>
+      </c>
+      <c r="H7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>602.44182699999999</v>
+      </c>
+      <c r="I7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>4.933268</v>
+      </c>
+      <c r="J7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>5.8589130000000003</v>
+      </c>
+      <c r="K7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>49.631498000000001</v>
+      </c>
+      <c r="L7" s="6">
+        <f>VLOOKUP($A7,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>54.529333000000001</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2784,239 +2782,243 @@
         <f>VLOOKUP($A8,raw!$A:$S,18,FALSE)</f>
         <v>3769464</v>
       </c>
-      <c r="E8">
-        <f>VLOOKUP($A8,raw!$A:$S,2,FALSE)</f>
-        <v>11452208</v>
-      </c>
-      <c r="F8">
-        <f>VLOOKUP($A8,raw!$A:$S,11,FALSE)</f>
-        <v>4842575</v>
-      </c>
-      <c r="G8">
-        <f>VLOOKUP($A8,raw!$A:$S,4,FALSE)</f>
-        <v>451959024</v>
-      </c>
-      <c r="H8">
-        <f>VLOOKUP($A8,raw!$A:$S,13,FALSE)</f>
-        <v>593442418</v>
-      </c>
-      <c r="I8">
-        <f>VLOOKUP($A8,raw!$A:$S,7,FALSE)</f>
-        <v>787272</v>
-      </c>
-      <c r="J8">
-        <f>VLOOKUP($A8,raw!$A:$S,16,FALSE)</f>
-        <v>935412</v>
-      </c>
-      <c r="K8">
-        <f>VLOOKUP($A8,raw!$A:$S,9,FALSE)</f>
-        <v>3081448</v>
-      </c>
-      <c r="L8">
-        <f>VLOOKUP($A8,raw!$A:$S,17,FALSE)</f>
-        <v>53786213</v>
+      <c r="E8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>11.452208000000001</v>
+      </c>
+      <c r="F8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>4.8425750000000001</v>
+      </c>
+      <c r="G8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>451.959024</v>
+      </c>
+      <c r="H8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>593.44241799999998</v>
+      </c>
+      <c r="I8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>4.8017339999999997</v>
+      </c>
+      <c r="J8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>5.760732</v>
+      </c>
+      <c r="K8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>49.143239000000001</v>
+      </c>
+      <c r="L8" s="6">
+        <f>VLOOKUP($A8,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>53.786212999999996</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C9" s="5"/>
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5">
+        <f>VLOOKUP($A9,raw!$A:$S,9,FALSE)</f>
+        <v>596144</v>
+      </c>
+      <c r="D9">
+        <f>VLOOKUP($A9,raw!$A:$S,18,FALSE)</f>
+        <v>713304</v>
+      </c>
+      <c r="E9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>2.474818</v>
+      </c>
+      <c r="F9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>1.2157169999999999</v>
+      </c>
+      <c r="G9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>79.102241000000006</v>
+      </c>
+      <c r="H9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>115.228326</v>
+      </c>
+      <c r="I9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>1.164191</v>
+      </c>
+      <c r="J9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>1.3083769999999999</v>
+      </c>
+      <c r="K9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>8.1751839999999998</v>
+      </c>
+      <c r="L9" s="6">
+        <f>VLOOKUP($A9,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>12.06476</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
       </c>
       <c r="C10" s="5">
         <f>VLOOKUP($A10,raw!$A:$S,9,FALSE)</f>
-        <v>596144</v>
+        <v>150540</v>
       </c>
       <c r="D10">
         <f>VLOOKUP($A10,raw!$A:$S,18,FALSE)</f>
-        <v>713304</v>
-      </c>
-      <c r="E10">
-        <f>VLOOKUP($A10,raw!$A:$S,2,FALSE)</f>
-        <v>2474818</v>
-      </c>
-      <c r="F10">
-        <f>VLOOKUP($A10,raw!$A:$S,11,FALSE)</f>
-        <v>1215717</v>
-      </c>
-      <c r="G10">
-        <f>VLOOKUP($A10,raw!$A:$S,4,FALSE)</f>
-        <v>79102241</v>
-      </c>
-      <c r="H10">
-        <f>VLOOKUP($A10,raw!$A:$S,13,FALSE)</f>
-        <v>115228326</v>
-      </c>
-      <c r="I10">
-        <f>VLOOKUP($A10,raw!$A:$S,7,FALSE)</f>
-        <v>161992</v>
-      </c>
-      <c r="J10">
-        <f>VLOOKUP($A10,raw!$A:$S,16,FALSE)</f>
-        <v>178532</v>
-      </c>
-      <c r="K10">
-        <f>VLOOKUP($A10,raw!$A:$S,9,FALSE)</f>
-        <v>596144</v>
-      </c>
-      <c r="L10">
-        <f>VLOOKUP($A10,raw!$A:$S,17,FALSE)</f>
-        <v>12064760</v>
+        <v>173340</v>
+      </c>
+      <c r="E10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>0.76018399999999997</v>
+      </c>
+      <c r="F10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>0.45746700000000001</v>
+      </c>
+      <c r="G10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>19.229776999999999</v>
+      </c>
+      <c r="H10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>27.638508999999999</v>
+      </c>
+      <c r="I10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>0.41484199999999999</v>
+      </c>
+      <c r="J10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>0.40828599999999998</v>
+      </c>
+      <c r="K10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>2.184739</v>
+      </c>
+      <c r="L10" s="6">
+        <f>VLOOKUP($A10,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>3.140854</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5">
+        <f>VLOOKUP($A11,raw!$A:$S,9,FALSE)</f>
+        <v>14920</v>
+      </c>
+      <c r="D11">
+        <f>VLOOKUP($A11,raw!$A:$S,18,FALSE)</f>
+        <v>45612</v>
+      </c>
+      <c r="E11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>1.811952</v>
+      </c>
+      <c r="F11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>1.767571</v>
+      </c>
+      <c r="G11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>2.0795149999999998</v>
+      </c>
+      <c r="H11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>9.3964259999999999</v>
+      </c>
+      <c r="I11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>0.26312099999999999</v>
+      </c>
+      <c r="J11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>0.31263800000000003</v>
+      </c>
+      <c r="K11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>0.82185900000000001</v>
+      </c>
+      <c r="L11" s="6">
+        <f>VLOOKUP($A11,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>2.6340379999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="5">
         <f>VLOOKUP($A12,raw!$A:$S,9,FALSE)</f>
-        <v>150540</v>
+        <v>39348</v>
       </c>
       <c r="D12">
         <f>VLOOKUP($A12,raw!$A:$S,18,FALSE)</f>
-        <v>173340</v>
-      </c>
-      <c r="E12">
-        <f>VLOOKUP($A12,raw!$A:$S,2,FALSE)</f>
-        <v>760184</v>
-      </c>
-      <c r="F12">
-        <f>VLOOKUP($A12,raw!$A:$S,11,FALSE)</f>
-        <v>457467</v>
-      </c>
-      <c r="G12">
-        <f>VLOOKUP($A12,raw!$A:$S,4,FALSE)</f>
-        <v>19229777</v>
-      </c>
-      <c r="H12">
-        <f>VLOOKUP($A12,raw!$A:$S,13,FALSE)</f>
-        <v>27638509</v>
-      </c>
-      <c r="I12">
-        <f>VLOOKUP($A12,raw!$A:$S,7,FALSE)</f>
-        <v>44872</v>
-      </c>
-      <c r="J12">
-        <f>VLOOKUP($A12,raw!$A:$S,16,FALSE)</f>
-        <v>48528</v>
-      </c>
-      <c r="K12">
-        <f>VLOOKUP($A12,raw!$A:$S,9,FALSE)</f>
-        <v>150540</v>
-      </c>
-      <c r="L12">
-        <f>VLOOKUP($A12,raw!$A:$S,17,FALSE)</f>
-        <v>3140854</v>
+        <v>789120</v>
+      </c>
+      <c r="E12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,2,FALSE)/(1000*1000)</f>
+        <v>7.8250539999999997</v>
+      </c>
+      <c r="F12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,11,FALSE)/(1000*1000)</f>
+        <v>2.62608</v>
+      </c>
+      <c r="G12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,4,FALSE)/(1000*1000)</f>
+        <v>0.98872099999999996</v>
+      </c>
+      <c r="H12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,13,FALSE)/(1000*1000)</f>
+        <v>196.001992</v>
+      </c>
+      <c r="I12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,6,FALSE)/(1000*1000)</f>
+        <v>0.25569799999999998</v>
+      </c>
+      <c r="J12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,15,FALSE)/(1000*1000)</f>
+        <v>1.0124979999999999</v>
+      </c>
+      <c r="K12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,8,FALSE)/(1000*1000)</f>
+        <v>0.46556799999999998</v>
+      </c>
+      <c r="L12" s="6">
+        <f>VLOOKUP($A12,raw!$A:$S,17,FALSE)/(1000*1000)</f>
+        <v>19.932639000000002</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="5">
-        <f>VLOOKUP($A13,raw!$A:$S,9,FALSE)</f>
-        <v>14920</v>
-      </c>
-      <c r="D13">
-        <f>VLOOKUP($A13,raw!$A:$S,18,FALSE)</f>
-        <v>45612</v>
-      </c>
-      <c r="E13">
-        <f>VLOOKUP($A13,raw!$A:$S,2,FALSE)</f>
-        <v>1811952</v>
-      </c>
-      <c r="F13">
-        <f>VLOOKUP($A13,raw!$A:$S,11,FALSE)</f>
-        <v>1767571</v>
-      </c>
-      <c r="G13">
-        <f>VLOOKUP($A13,raw!$A:$S,4,FALSE)</f>
-        <v>2079515</v>
-      </c>
-      <c r="H13">
-        <f>VLOOKUP($A13,raw!$A:$S,13,FALSE)</f>
-        <v>9396426</v>
-      </c>
-      <c r="I13">
-        <f>VLOOKUP($A13,raw!$A:$S,7,FALSE)</f>
-        <v>4124</v>
-      </c>
-      <c r="J13">
-        <f>VLOOKUP($A13,raw!$A:$S,16,FALSE)</f>
-        <v>13580</v>
-      </c>
-      <c r="K13">
-        <f>VLOOKUP($A13,raw!$A:$S,9,FALSE)</f>
-        <v>14920</v>
-      </c>
-      <c r="L13">
-        <f>VLOOKUP($A13,raw!$A:$S,17,FALSE)</f>
-        <v>2634038</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="5">
-        <f>VLOOKUP($A14,raw!$A:$S,9,FALSE)</f>
-        <v>39348</v>
-      </c>
-      <c r="D14">
-        <f>VLOOKUP($A14,raw!$A:$S,18,FALSE)</f>
-        <v>789120</v>
-      </c>
-      <c r="E14">
-        <f>VLOOKUP($A14,raw!$A:$S,2,FALSE)</f>
-        <v>7825054</v>
-      </c>
-      <c r="F14">
-        <f>VLOOKUP($A14,raw!$A:$S,11,FALSE)</f>
-        <v>2626080</v>
-      </c>
-      <c r="G14">
-        <f>VLOOKUP($A14,raw!$A:$S,4,FALSE)</f>
-        <v>988721</v>
-      </c>
-      <c r="H14">
-        <f>VLOOKUP($A14,raw!$A:$S,13,FALSE)</f>
-        <v>196001992</v>
-      </c>
-      <c r="I14">
-        <f>VLOOKUP($A14,raw!$A:$S,7,FALSE)</f>
-        <v>4888</v>
-      </c>
-      <c r="J14">
-        <f>VLOOKUP($A14,raw!$A:$S,16,FALSE)</f>
-        <v>167204</v>
-      </c>
-      <c r="K14">
-        <f>VLOOKUP($A14,raw!$A:$S,9,FALSE)</f>
-        <v>39348</v>
-      </c>
-      <c r="L14">
-        <f>VLOOKUP($A14,raw!$A:$S,17,FALSE)</f>
-        <v>19932639</v>
-      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>